<commit_message>
Fix col:branchlength type and change dataset type enum
</commit_message>
<xml_diff>
--- a/webservice/src/test/resources/xls/Torotrogla_villosa.xlsx
+++ b/webservice/src/test/resources/xls/Torotrogla_villosa.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markus/code/col/backend/webservice/src/test/resources/xls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B50F0F-7BCC-EF47-AFC0-680C35E01E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DCF526-09F7-A246-B18F-FFFFB1D6FBF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="8620" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="NameUsage" sheetId="4" r:id="rId1"/>
-    <sheet name="Reference" sheetId="2" r:id="rId2"/>
-    <sheet name="TypeMaterial" sheetId="5" r:id="rId3"/>
+    <sheet name="Name" sheetId="6" r:id="rId1"/>
+    <sheet name="Taxon" sheetId="4" r:id="rId2"/>
+    <sheet name="Synonym" sheetId="7" r:id="rId3"/>
+    <sheet name="Reference" sheetId="2" r:id="rId4"/>
+    <sheet name="TypeMaterial" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
   <si>
     <t>Picobia</t>
   </si>
@@ -57,9 +59,6 @@
     <t>reject Trouessart's synonymy</t>
   </si>
   <si>
-    <t>considered synonym of Syringophilus bipectinatus</t>
-  </si>
-  <si>
     <t>Torotrogla</t>
   </si>
   <si>
@@ -129,9 +128,6 @@
     <t>basionymID</t>
   </si>
   <si>
-    <t>status</t>
-  </si>
-  <si>
     <t>rank</t>
   </si>
   <si>
@@ -144,10 +140,7 @@
     <t>specificEpithet</t>
   </si>
   <si>
-    <t>namePublishedInYear</t>
-  </si>
-  <si>
-    <t>namePublishedInPage</t>
+    <t>referenceID</t>
   </si>
   <si>
     <t>remarks</t>
@@ -198,9 +191,6 @@
     <t>accordingToID</t>
   </si>
   <si>
-    <t>nameReferenceID</t>
-  </si>
-  <si>
     <t>(Hancock, 1895)</t>
   </si>
   <si>
@@ -210,16 +200,13 @@
     <t>species</t>
   </si>
   <si>
-    <t>synonym</t>
-  </si>
-  <si>
     <t>72590-acc</t>
   </si>
   <si>
-    <t>Syringophilus</t>
-  </si>
-  <si>
-    <t>bipectinatus</t>
+    <t>publishedInYear</t>
+  </si>
+  <si>
+    <t>publishedInPage</t>
   </si>
 </sst>
 </file>
@@ -332,7 +319,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -361,9 +348,6 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -710,274 +694,119 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11600BE0-8666-EE4B-82A9-E363F7D1406E}">
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="24"/>
-    <col min="2" max="2" width="9.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="23" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="58.140625" style="8" customWidth="1"/>
-    <col min="16" max="16384" width="10.7109375" style="8"/>
+    <col min="1" max="1" width="10.7109375" style="23"/>
+    <col min="2" max="2" width="12.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="22" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="58.140625" style="8" customWidth="1"/>
+    <col min="11" max="16384" width="10.7109375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="22" t="s">
+    <row r="1" spans="1:10" s="16" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="G1" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="J1" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" s="17" t="s">
+    </row>
+    <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="18">
+        <v>1922</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="M1" s="17" t="s">
+      <c r="E2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="9">
+        <v>1895</v>
+      </c>
+      <c r="H2" s="11">
+        <v>384</v>
+      </c>
+      <c r="I2" s="12">
+        <v>189500107</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="18">
+        <v>63439</v>
+      </c>
+      <c r="B3" s="18">
+        <v>1922</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="N1" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="O1" s="17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="19">
-        <v>1922</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="10" t="s">
+      <c r="D3" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="9">
-        <v>1895</v>
-      </c>
-      <c r="K2" s="11">
-        <v>384</v>
-      </c>
-      <c r="L2" s="12">
-        <v>189500107</v>
-      </c>
-      <c r="M2" s="12">
-        <v>189500107</v>
-      </c>
-      <c r="N2" s="11">
-        <v>384</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="19">
-        <v>86921</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3" s="9">
-        <v>1895</v>
-      </c>
-      <c r="K3" s="11"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12">
-        <v>189500109</v>
-      </c>
-      <c r="N3" s="11">
-        <v>866</v>
-      </c>
-      <c r="O3" s="13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="J4" s="9"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="13"/>
-    </row>
-    <row r="5" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="19">
-        <v>72590</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" s="9">
-        <v>1895</v>
-      </c>
-      <c r="K5" s="11"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12">
-        <v>189500304</v>
-      </c>
-      <c r="N5" s="11">
-        <v>682</v>
-      </c>
-      <c r="O5" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="19">
-        <v>63439</v>
-      </c>
-      <c r="C6" s="19">
-        <v>1922</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" s="10" t="s">
+      <c r="G3" s="9">
+        <v>1970</v>
+      </c>
+      <c r="H3" s="11">
+        <v>30</v>
+      </c>
+      <c r="I3" s="12">
+        <v>197000593</v>
+      </c>
+      <c r="J3" s="13" t="s">
         <v>8</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J6" s="9">
-        <v>1970</v>
-      </c>
-      <c r="K6" s="11">
-        <v>30</v>
-      </c>
-      <c r="L6" s="12">
-        <v>197000593</v>
-      </c>
-      <c r="M6" s="12">
-        <v>197000593</v>
-      </c>
-      <c r="N6" s="11">
-        <v>30</v>
-      </c>
-      <c r="O6" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="20">
-        <v>63440</v>
-      </c>
-      <c r="C7" s="23">
-        <v>1922</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="J7" s="9">
-        <v>1970</v>
-      </c>
-      <c r="K7" s="15"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12">
-        <v>197600211</v>
-      </c>
-      <c r="N7" s="15">
-        <v>156</v>
-      </c>
-      <c r="O7" s="13" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -987,6 +816,172 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" style="23"/>
+    <col min="2" max="2" width="14.140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.140625" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="10.7109375" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="16" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="18">
+        <v>1922</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="12">
+        <v>189500107</v>
+      </c>
+      <c r="D2" s="11">
+        <v>384</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="18">
+        <v>86921</v>
+      </c>
+      <c r="C3" s="12">
+        <v>189500109</v>
+      </c>
+      <c r="D3" s="11">
+        <v>866</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="12">
+        <v>189500304</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="13"/>
+    </row>
+    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="18">
+        <v>63439</v>
+      </c>
+      <c r="C5" s="12">
+        <v>197000593</v>
+      </c>
+      <c r="D5" s="11">
+        <v>30</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="19">
+        <v>63440</v>
+      </c>
+      <c r="C6" s="12">
+        <v>197600211</v>
+      </c>
+      <c r="D6" s="14">
+        <v>156</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0D6B9EC-29BC-0147-B692-54009A8011B0}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" style="23"/>
+    <col min="2" max="2" width="9.28515625" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.140625" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="10.7109375" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="16" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="18">
+        <v>72590</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="12">
+        <v>189500304</v>
+      </c>
+      <c r="D2" s="11">
+        <v>682</v>
+      </c>
+      <c r="E2" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
@@ -1011,129 +1006,129 @@
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="24">
+        <v>189500107</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="25">
-        <v>189500107</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>44</v>
+      <c r="C2" s="24" t="s">
+        <v>41</v>
       </c>
       <c r="D2" s="3">
         <v>1895</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="G2" s="3">
         <v>29</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="25">
+      <c r="A3" s="24">
         <v>189500109</v>
       </c>
-      <c r="B3" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>44</v>
+      <c r="B3" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>41</v>
       </c>
       <c r="D3" s="3">
         <v>1895</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="G3" s="3">
         <v>29</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="25">
+      <c r="A4" s="24">
         <v>189500304</v>
       </c>
-      <c r="B4" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>45</v>
+      <c r="B4" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>42</v>
       </c>
       <c r="D4" s="3">
         <v>1895</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4" s="3">
         <v>29</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="25">
+      <c r="A5" s="24">
         <v>197000593</v>
       </c>
-      <c r="B5" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>46</v>
+      <c r="B5" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>43</v>
       </c>
       <c r="D5" s="3">
         <v>1970</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="G5" s="3">
         <v>5</v>
@@ -1142,27 +1137,27 @@
         <v>6</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="25">
+      <c r="A6" s="24">
         <v>197600211</v>
       </c>
-      <c r="B6" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>47</v>
+      <c r="B6" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>44</v>
       </c>
       <c r="D6" s="3">
         <v>1976</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="G6" s="3">
         <v>1</v>
@@ -1171,7 +1166,7 @@
         <v>4</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1183,7 +1178,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1200,26 +1195,26 @@
   <sheetData>
     <row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B2" s="19">
+      <c r="B2" s="18">
         <v>1922</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="18" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adjust names index store tests for stricter checks on canonicalID
</commit_message>
<xml_diff>
--- a/webservice/src/test/resources/xls/Torotrogla_villosa.xlsx
+++ b/webservice/src/test/resources/xls/Torotrogla_villosa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markus/code/col/backend/webservice/src/test/resources/xls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DCF526-09F7-A246-B18F-FFFFB1D6FBF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC6E39D-50F8-0947-BABE-19EDC71A9764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6360" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Name" sheetId="6" r:id="rId1"/>

</xml_diff>